<commit_message>
Test queries updated slightly, fixed requery bug
</commit_message>
<xml_diff>
--- a/jasmine/Test Data/Test Queries.xlsx
+++ b/jasmine/Test Data/Test Queries.xlsx
@@ -107,9 +107,6 @@
     <t>(9123wfedsv4.245) JPYsgrwg DKK 2-3-2009</t>
   </si>
   <si>
-    <t>(987) DKK HUF 12-12-20012</t>
-  </si>
-  <si>
     <t>(987) DKK HUF gscx 12-12-20012</t>
   </si>
   <si>
@@ -131,10 +128,13 @@
     <t xml:space="preserve">    (91234.245gsfxc)    JPY   DKK   2-3-2009     </t>
   </si>
   <si>
-    <t xml:space="preserve">   (987)     DKK     HUF           12-12-20012     </t>
-  </si>
-  <si>
     <t xml:space="preserve">   (987)     DKK     HUF           12 12 20012     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">   (987)     DKK     HUF           12-12-2012     </t>
+  </si>
+  <si>
+    <t>(987) DKK HUF 12-12-2012</t>
   </si>
 </sst>
 </file>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,34 +594,34 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" t="s">
         <v>27</v>
-      </c>
-      <c r="C20" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" t="s">
         <v>29</v>
-      </c>
-      <c r="C22" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="C23" t="s">
         <v>31</v>
-      </c>
-      <c r="C23" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
         <v>33</v>
-      </c>
-      <c r="C24" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -629,7 +629,7 @@
         <v>35</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test Queries updated slighly due to bug found in it
</commit_message>
<xml_diff>
--- a/jasmine/Test Data/Test Queries.xlsx
+++ b/jasmine/Test Data/Test Queries.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Valid Queries</t>
   </si>
@@ -135,6 +135,9 @@
   </si>
   <si>
     <t>(987) DKK HUF 12-12-2012</t>
+  </si>
+  <si>
+    <t>(1234.23425) GBP DKgsfvK</t>
   </si>
 </sst>
 </file>
@@ -454,8 +457,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -525,7 +528,7 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>